<commit_message>
Dry run works without wildcards for Excel output
</commit_message>
<xml_diff>
--- a/input/positions_by_lineage_and_segment.xlsx
+++ b/input/positions_by_lineage_and_segment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nic/NIC/Berlin/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD88784-A4A3-0243-BC98-F832468763DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDF6145-57F3-AC40-A160-6D031F719E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{C39EC7A6-78BA-FA40-9ADF-13729B2CB2F0}"/>
   </bookViews>
@@ -48,7 +48,7 @@
     <t>h1n1pdm</t>
   </si>
   <si>
-    <t>na</t>
+    <t>pa</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A121" sqref="A121:C133"/>
+      <selection pane="bottomLeft" activeCell="F135" sqref="F135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Snakefile now runs rules nextalign and get_positions together :)
</commit_message>
<xml_diff>
--- a/input/positions_by_lineage_and_segment.xlsx
+++ b/input/positions_by_lineage_and_segment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nic/NIC/Berlin/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DDF6145-57F3-AC40-A160-6D031F719E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0360857-7E3D-7940-B33D-0AF6400F08A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{C39EC7A6-78BA-FA40-9ADF-13729B2CB2F0}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="9">
   <si>
     <t>lineage</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>pa</t>
+  </si>
+  <si>
+    <t>np</t>
   </si>
 </sst>
 </file>
@@ -419,11 +422,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D60660FF-393D-EF41-9AB5-5972F77FF57E}">
-  <dimension ref="A1:C133"/>
+  <dimension ref="A1:C139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F135" sqref="F135"/>
+      <selection pane="bottomLeft" activeCell="A134" sqref="A134:C139"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1894,6 +1897,72 @@
         <v>45</v>
       </c>
     </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A134" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B134" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C134" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A135" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C135" s="1">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A136" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B136" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C136" s="1">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A137" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C137" s="1">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A138" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B138" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C138" s="1">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A139" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C139" s="1">
+        <v>263</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>